<commit_message>
Commit before Merge 5/22
</commit_message>
<xml_diff>
--- a/LyndaTestAutomationFramework/LyndaTestAutomationFramework/Tests/General/Tests/BVT5/TestData/Public_lpAcctData.xlsx
+++ b/LyndaTestAutomationFramework/LyndaTestAutomationFramework/Tests/General/Tests/BVT5/TestData/Public_lpAcctData.xlsx
@@ -48,26 +48,34 @@
     <t>TestFname-d@mailinator.com</t>
   </si>
   <si>
-    <t>lpuser-5-17-2012-55347</t>
-  </si>
-  <si>
-    <t>lpuser-5-17-2012-55493</t>
-  </si>
-  <si>
-    <t>lpuser-5-21-2012-38339</t>
-  </si>
-  <si>
-    <t>lpuser-5-21-2012-38363</t>
+    <t>lpuser-5-22-2012-59800</t>
+  </si>
+  <si>
+    <t>lpuser-5-22-2012-59840</t>
+  </si>
+  <si>
+    <t>lpuser-5-22-2012-59876</t>
+  </si>
+  <si>
+    <t>lpuser-5-22-2012-59911</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -90,13 +98,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -399,7 +410,7 @@
   <dimension ref="B1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,9 +438,9 @@
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>38144</v>
-      </c>
-      <c r="C2" t="s">
+        <v>38165</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
@@ -441,7 +452,7 @@
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>38144</v>
+        <v>38165</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -450,12 +461,12 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>38144</v>
+        <v>38165</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -464,12 +475,12 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>38144</v>
+        <v>38165</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -478,10 +489,13 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Commit before pushing to branchjude 5/23
</commit_message>
<xml_diff>
--- a/LyndaTestAutomationFramework/LyndaTestAutomationFramework/Tests/General/Tests/BVT5/TestData/Public_lpAcctData.xlsx
+++ b/LyndaTestAutomationFramework/LyndaTestAutomationFramework/Tests/General/Tests/BVT5/TestData/Public_lpAcctData.xlsx
@@ -48,16 +48,16 @@
     <t>TestFname-d@mailinator.com</t>
   </si>
   <si>
-    <t>lpuser-5-22-2012-59800</t>
-  </si>
-  <si>
-    <t>lpuser-5-22-2012-59840</t>
-  </si>
-  <si>
-    <t>lpuser-5-22-2012-59876</t>
-  </si>
-  <si>
-    <t>lpuser-5-22-2012-59911</t>
+    <t>lpuser-5-23-2012-55611</t>
+  </si>
+  <si>
+    <t>lpuser-5-23-2012-55645</t>
+  </si>
+  <si>
+    <t>lpuser-5-23-2012-55681</t>
+  </si>
+  <si>
+    <t>lpuser-5-23-2012-55713</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>38165</v>
+        <v>38174</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
@@ -452,7 +452,7 @@
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>38165</v>
+        <v>38174</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -466,7 +466,7 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>38165</v>
+        <v>38174</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -480,7 +480,7 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>38165</v>
+        <v>38174</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>

</xml_diff>